<commit_message>
CF for hydro - all CFs done
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B45D1FC-2B03-4D74-B877-2E99B55C0262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06CE1B8-99A9-453F-8DA9-A888E4CE2831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodity_labels" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="105">
   <si>
     <t>p</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>Used for CF Growth Only Data is region dependent and represented in python code Class 8</t>
+  </si>
+  <si>
+    <t>HYDRO</t>
   </si>
 </sst>
 </file>
@@ -925,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B94D054-32A6-4BDE-98D7-472A0F6D7282}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB57A83-05BB-4B3C-8DF8-E9284C1E7CDB}">
-  <dimension ref="A1:AK20"/>
+  <dimension ref="A1:AK22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4185,6 +4188,232 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="R21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="S21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="T21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="U21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="V21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="W21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="X21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Y21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Z21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AB21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AC21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AD21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AE21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AF21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AG21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AH21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AI21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AJ21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AK21" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="R22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="S22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="T22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="U22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="V22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="W22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="X22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Y22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Z22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AA22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AB22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AC22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AD22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AE22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AF22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AG22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AH22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AI22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AJ22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AK22" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Build SQL and SQLite files
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923068B-82D8-4C87-9362-D2BD9E5E59C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A84468F-7BED-4EA0-8291-8C7E6769B125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5130" yWindow="5295" windowWidth="21015" windowHeight="10200" tabRatio="849" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodity_labels" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="196">
   <si>
     <t>p</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>maxact_notes</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
 </sst>
 </file>
@@ -2456,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0904B615-50FA-4F82-9A22-035234CBED38}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2480,7 +2483,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="B2" s="1">
         <v>0.17</v>
@@ -14423,7 +14426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9C1FD3-1933-4825-94FA-30ED0724E508}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix Bugs shown during TEMOA run
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A84468F-7BED-4EA0-8291-8C7E6769B125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C8BFAB-9F8F-4460-A8C4-E63D655DF403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="5295" windowWidth="21015" windowHeight="10200" tabRatio="849" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodity_labels" sheetId="1" r:id="rId1"/>
@@ -2459,7 +2459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0904B615-50FA-4F82-9A22-035234CBED38}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2501,7 +2501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FBD8C2-7885-48CF-A6D2-8373F214E00B}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2786,7 +2786,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2959,7 +2959,7 @@
   <dimension ref="A1:AL71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="E3" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -11183,7 +11183,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A23:A25"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
First Successful run Temoa before lim cap
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C8BFAB-9F8F-4460-A8C4-E63D655DF403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498A4D3D-328A-451C-B3FB-5DA8E8125FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodity_labels" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="195">
   <si>
     <t>p</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Petroleum</t>
-  </si>
-  <si>
-    <t>LanfillGas</t>
   </si>
   <si>
     <t>LandfillGas</t>
@@ -1905,7 +1902,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1959,10 +1956,10 @@
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1973,7 +1970,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1984,18 +1981,18 @@
         <v>0.90800000000000003</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="4">
         <v>0.87390000000000001</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2006,7 +2003,7 @@
         <v>0.87390000000000001</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2017,7 +2014,7 @@
         <v>0.87390000000000001</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2028,7 +2025,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2039,18 +2036,18 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="4">
         <v>0.88249999999999995</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2061,7 +2058,7 @@
         <v>0.88249999999999995</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2072,7 +2069,7 @@
         <v>0.88249999999999995</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2083,7 +2080,7 @@
         <v>0.97840000000000005</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2094,7 +2091,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2105,7 +2102,7 @@
         <v>0.29199999999999998</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2116,7 +2113,7 @@
         <v>0.94210000000000005</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2127,7 +2124,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2138,7 +2135,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2149,7 +2146,7 @@
         <v>0.88249999999999995</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2160,7 +2157,7 @@
         <v>0.88249999999999995</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2171,73 +2168,73 @@
         <v>0.88249999999999995</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" s="4">
         <v>0.88249999999999995</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B22" s="4">
         <v>0.88249999999999995</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="4">
         <v>0.88249999999999995</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" s="4">
         <v>0.88249999999999995</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" s="4">
         <v>0.90800000000000003</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B26" s="4">
         <v>0.90800000000000003</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2248,7 +2245,7 @@
         <v>0.90800000000000003</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2259,7 +2256,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2270,7 +2267,7 @@
         <v>0.97840000000000005</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2281,7 +2278,7 @@
         <v>0.97840000000000005</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2292,7 +2289,7 @@
         <v>0.29199999999999998</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2303,7 +2300,7 @@
         <v>0.94210000000000005</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2314,7 +2311,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2325,7 +2322,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2336,7 +2333,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2347,7 +2344,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2358,29 +2355,29 @@
         <v>0.39500000000000002</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" s="4">
         <v>0.39500000000000002</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" s="4">
         <v>0.39500000000000002</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2391,7 +2388,7 @@
         <v>0.7</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2402,7 +2399,7 @@
         <v>0.7</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2413,7 +2410,7 @@
         <v>0.7</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2424,7 +2421,7 @@
         <v>0.7</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2435,7 +2432,7 @@
         <v>0.7</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2446,7 +2443,7 @@
         <v>0.7</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2472,24 +2469,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1">
         <v>0.17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2501,7 +2498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FBD8C2-7885-48CF-A6D2-8373F214E00B}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2515,7 +2512,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2523,7 +2520,7 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2531,7 +2528,7 @@
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2539,7 +2536,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2547,23 +2544,23 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2571,7 +2568,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2579,7 +2576,7 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2587,7 +2584,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2611,22 +2608,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
         <v>182</v>
-      </c>
-      <c r="B1" t="s">
-        <v>183</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" t="s">
         <v>184</v>
-      </c>
-      <c r="E1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2649,22 +2646,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
         <v>182</v>
-      </c>
-      <c r="B1" t="s">
-        <v>183</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" t="s">
         <v>186</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>187</v>
-      </c>
-      <c r="F1" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2687,22 +2684,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
         <v>182</v>
-      </c>
-      <c r="B1" t="s">
-        <v>183</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" t="s">
         <v>192</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>193</v>
-      </c>
-      <c r="F1" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2722,22 +2719,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
         <v>182</v>
-      </c>
-      <c r="B1" t="s">
-        <v>183</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>190</v>
-      </c>
-      <c r="F1" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2761,19 +2758,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
         <v>179</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>180</v>
-      </c>
-      <c r="E1" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2786,7 +2783,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2907,46 +2904,46 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2958,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B94D054-32A6-4BDE-98D7-472A0F6D7282}">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2976,13 +2973,13 @@
   <sheetData>
     <row r="1" spans="1:38" s="11" customFormat="1">
       <c r="A1" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>10</v>
@@ -3098,10 +3095,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>27</v>
@@ -3214,10 +3211,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>29</v>
@@ -3330,10 +3327,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>39</v>
@@ -3446,10 +3443,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>43</v>
@@ -3562,10 +3559,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>44</v>
@@ -3678,10 +3675,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>32</v>
@@ -3794,10 +3791,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>33</v>
@@ -3910,13 +3907,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>62</v>
@@ -4026,10 +4023,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>36</v>
@@ -4142,10 +4139,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>37</v>
@@ -4258,13 +4255,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>68</v>
@@ -4374,10 +4371,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>30</v>
@@ -4490,10 +4487,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>31</v>
@@ -4606,10 +4603,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>28</v>
@@ -4942,7 +4939,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>60</v>
@@ -5052,7 +5049,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>60</v>
@@ -6922,7 +6919,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>47</v>
@@ -6931,7 +6928,7 @@
         <v>52</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H36" s="4">
         <f>1-0.021</f>
@@ -7066,16 +7063,16 @@
         <v>6</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H37" s="4">
         <f>(1-0.021*1.53)</f>
@@ -7204,19 +7201,19 @@
     </row>
     <row r="38" spans="1:38">
       <c r="A38" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>52</v>
@@ -7317,19 +7314,19 @@
     </row>
     <row r="39" spans="1:38">
       <c r="A39" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>52</v>
@@ -7430,19 +7427,19 @@
     </row>
     <row r="40" spans="1:38">
       <c r="A40" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>52</v>
@@ -7546,13 +7543,13 @@
         <v>6</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>19</v>
@@ -7662,13 +7659,13 @@
         <v>6</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>19</v>
@@ -7778,13 +7775,13 @@
         <v>6</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>19</v>
@@ -7894,13 +7891,13 @@
         <v>6</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>18</v>
@@ -8010,13 +8007,13 @@
         <v>6</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>18</v>
@@ -8126,13 +8123,13 @@
         <v>6</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>18</v>
@@ -8242,13 +8239,13 @@
         <v>6</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>20</v>
@@ -8358,13 +8355,13 @@
         <v>6</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>20</v>
@@ -8474,13 +8471,13 @@
         <v>6</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>20</v>
@@ -8590,16 +8587,16 @@
         <v>6</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>62</v>
@@ -8706,16 +8703,16 @@
         <v>6</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>62</v>
@@ -8822,16 +8819,16 @@
         <v>6</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>62</v>
@@ -8938,16 +8935,16 @@
         <v>6</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>62</v>
@@ -9054,16 +9051,16 @@
         <v>6</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>62</v>
@@ -9170,16 +9167,16 @@
         <v>6</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>62</v>
@@ -9286,16 +9283,16 @@
         <v>6</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>62</v>
@@ -9402,16 +9399,16 @@
         <v>6</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>62</v>
@@ -9518,16 +9515,16 @@
         <v>6</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>62</v>
@@ -9634,16 +9631,16 @@
         <v>6</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>62</v>
@@ -9750,16 +9747,16 @@
         <v>6</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>62</v>
@@ -9866,16 +9863,16 @@
         <v>6</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>62</v>
@@ -9982,13 +9979,13 @@
         <v>6</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>16</v>
@@ -10098,13 +10095,13 @@
         <v>6</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>16</v>
@@ -10214,13 +10211,13 @@
         <v>6</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>16</v>
@@ -10330,16 +10327,16 @@
         <v>6</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>56</v>
@@ -10446,16 +10443,16 @@
         <v>6</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>56</v>
@@ -10562,16 +10559,16 @@
         <v>6</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>56</v>
@@ -10678,16 +10675,16 @@
         <v>6</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>56</v>
@@ -10794,16 +10791,16 @@
         <v>6</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>56</v>
@@ -10910,16 +10907,16 @@
         <v>6</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>56</v>
@@ -11029,10 +11026,10 @@
         <v>6</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>15</v>
@@ -11199,13 +11196,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -11213,10 +11210,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D2" s="8">
         <v>118.6</v>
@@ -11227,10 +11224,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D3" s="8">
         <v>118.62</v>
@@ -11241,10 +11238,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D4" s="8">
         <v>118.62</v>
@@ -11252,13 +11249,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D5" s="8">
         <v>5.95</v>
@@ -11266,13 +11263,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D6" s="8">
         <v>5.95</v>
@@ -11280,13 +11277,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D7" s="8">
         <v>3.56</v>
@@ -11294,13 +11291,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D8" s="8">
         <v>3.58</v>
@@ -11311,10 +11308,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D9" s="8">
         <v>202.32</v>
@@ -11322,13 +11319,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D10" s="8">
         <v>10.198</v>
@@ -11336,13 +11333,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D11" s="8">
         <v>2.1059999999999999</v>
@@ -11353,10 +11350,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D12" s="8">
         <v>0</v>
@@ -11367,10 +11364,10 @@
         <v>27</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D13" s="8">
         <v>0</v>
@@ -11381,10 +11378,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D14" s="8">
         <v>0</v>
@@ -11395,10 +11392,10 @@
         <v>39</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D15" s="8">
         <v>0</v>
@@ -11409,10 +11406,10 @@
         <v>43</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D16" s="8">
         <v>0</v>
@@ -11423,10 +11420,10 @@
         <v>44</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D17" s="8">
         <v>0</v>
@@ -11437,10 +11434,10 @@
         <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D18" s="8">
         <v>0</v>
@@ -11451,10 +11448,10 @@
         <v>33</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D19" s="8">
         <v>0</v>
@@ -11462,13 +11459,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D20" s="8">
         <v>119.41764496915395</v>
@@ -11479,10 +11476,10 @@
         <v>36</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D21" s="8">
         <v>119.41764496915395</v>
@@ -11493,10 +11490,10 @@
         <v>37</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D22" s="8">
         <v>119.41764496915395</v>
@@ -11504,13 +11501,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D23" s="8">
         <v>229.51879128207057</v>
@@ -11521,10 +11518,10 @@
         <v>30</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D24" s="8">
         <v>229.51879128207057</v>
@@ -11535,10 +11532,10 @@
         <v>31</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D25" s="8">
         <v>229.51879128207057</v>
@@ -11549,10 +11546,10 @@
         <v>28</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="D26" s="8">
         <v>214.12654767006592</v>
@@ -11746,18 +11743,18 @@
   <sheetData>
     <row r="1" spans="9:10">
       <c r="I1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="9:10">
       <c r="I3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="9:10">
@@ -11770,7 +11767,7 @@
     </row>
     <row r="5" spans="9:10">
       <c r="I5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J5" s="1">
         <v>35608740</v>
@@ -11778,7 +11775,7 @@
     </row>
     <row r="6" spans="9:10">
       <c r="I6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J6" s="1">
         <v>4263628</v>
@@ -11786,7 +11783,7 @@
     </row>
     <row r="7" spans="9:10">
       <c r="I7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J7" s="1">
         <v>7572266</v>
@@ -11794,7 +11791,7 @@
     </row>
     <row r="8" spans="9:10">
       <c r="I8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="1">
         <v>557186</v>
@@ -11802,7 +11799,7 @@
     </row>
     <row r="9" spans="9:10">
       <c r="I9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J9" s="1">
         <v>110398</v>
@@ -11810,7 +11807,7 @@
     </row>
     <row r="10" spans="9:10">
       <c r="I10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J10" s="1">
         <v>5710</v>
@@ -11818,7 +11815,7 @@
     </row>
     <row r="11" spans="9:10">
       <c r="I11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J11" s="1">
         <v>18396</v>
@@ -11826,7 +11823,7 @@
     </row>
     <row r="12" spans="9:10">
       <c r="I12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J12" s="1">
         <v>60238</v>
@@ -11834,7 +11831,7 @@
     </row>
     <row r="13" spans="9:10">
       <c r="I13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J13" s="1">
         <v>1465316</v>
@@ -11842,16 +11839,16 @@
     </row>
     <row r="17" spans="9:14">
       <c r="I17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="18" spans="9:14">
@@ -11870,7 +11867,7 @@
     </row>
     <row r="19" spans="9:14">
       <c r="I19" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J19" s="1">
         <v>80</v>
@@ -11898,16 +11895,16 @@
     </row>
     <row r="23" spans="9:14">
       <c r="I23" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="9:14">
@@ -11927,7 +11924,7 @@
     </row>
     <row r="25" spans="9:14">
       <c r="I25" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J25" s="1">
         <v>80</v>
@@ -11957,22 +11954,22 @@
     </row>
     <row r="29" spans="9:14">
       <c r="I29" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="L29" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="N29" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="9:14">
@@ -12001,7 +11998,7 @@
     </row>
     <row r="31" spans="9:14">
       <c r="I31" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J31" s="1">
         <f>SUM(J5:J7)</f>
@@ -12072,62 +12069,62 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1">
         <v>2030</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="1">
         <v>26505.0756</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="1">
         <v>2050</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -12157,19 +12154,19 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
@@ -12273,19 +12270,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" s="4">
         <v>0.15430339646551175</v>
@@ -12386,19 +12383,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G3" s="4">
         <v>0.1531866860427854</v>
@@ -12499,19 +12496,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="4">
         <v>0.15155102652611524</v>
@@ -12612,19 +12609,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" s="4">
         <v>0.15049311805235732</v>
@@ -12725,19 +12722,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="4">
         <v>0.15013521014437531</v>
@@ -12838,19 +12835,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G7" s="4">
         <v>0.14990328410944515</v>
@@ -12951,19 +12948,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" s="4">
         <v>0.215</v>
@@ -13064,19 +13061,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G9" s="4">
         <v>0.215</v>
@@ -13177,19 +13174,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" s="4">
         <v>0.215</v>
@@ -13293,16 +13290,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G11" s="4">
         <v>0.2145</v>
@@ -13403,16 +13400,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>60</v>
@@ -13516,16 +13513,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>60</v>
@@ -13629,16 +13626,16 @@
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>60</v>
@@ -13742,16 +13739,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>60</v>
@@ -13855,16 +13852,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>60</v>
@@ -13968,16 +13965,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>60</v>
@@ -14084,13 +14081,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>60</v>
@@ -14197,13 +14194,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>66</v>
@@ -14310,13 +14307,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>66</v>
@@ -14441,16 +14438,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -14530,7 +14527,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -14544,7 +14541,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -14573,13 +14570,13 @@
   <sheetData>
     <row r="1" spans="1:34" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D1" s="3">
         <v>2020</v>
@@ -14683,7 +14680,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" s="6">
         <v>6.5421499999999994E-2</v>
@@ -14784,10 +14781,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="6">
         <v>6.5421499999999994E-2</v>
@@ -14888,10 +14885,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" s="6">
         <v>6.5421499999999994E-2</v>
@@ -14995,7 +14992,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" s="6">
         <v>6.5421499999999994E-2</v>
@@ -15099,7 +15096,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D6" s="6">
         <v>6.5421499999999994E-2</v>
@@ -15203,7 +15200,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" s="6">
         <v>6.5421499999999994E-2</v>
@@ -15304,10 +15301,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="6">
         <v>6.5421499999999994E-2</v>
@@ -15408,10 +15405,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D9" s="6">
         <v>6.5421499999999994E-2</v>
@@ -15512,10 +15509,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" s="6">
         <v>6.5421499999999994E-2</v>
@@ -15616,10 +15613,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D11" s="6">
         <v>6.5421499999999994E-2</v>
@@ -15723,7 +15720,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D12" s="6">
         <v>6.5000000000000002E-2</v>
@@ -15827,7 +15824,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13" s="6">
         <v>6.5000000000000002E-2</v>
@@ -15931,7 +15928,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D14" s="6">
         <v>6.5000000000000002E-2</v>
@@ -16035,7 +16032,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D15" s="6">
         <v>6.5000000000000002E-2</v>
@@ -16139,7 +16136,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16" s="6">
         <v>5.7877100000000001E-2</v>
@@ -16243,7 +16240,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D17" s="6">
         <v>5.7877100000000001E-2</v>
@@ -16347,7 +16344,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D18" s="6">
         <v>5.6412210360996473E-2</v>
@@ -16451,7 +16448,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" s="6">
         <v>5.6698294578795688E-2</v>
@@ -16555,7 +16552,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" s="6">
         <v>5.2714068831298061E-2</v>
@@ -16659,7 +16656,7 @@
         <v>25</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D21" s="6">
         <v>5.4287470296592102E-2</v>
@@ -16763,7 +16760,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D22" s="6">
         <v>5.4287470296592102E-2</v>
@@ -16864,10 +16861,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D23" s="6">
         <v>7.1222518716689817E-2</v>
@@ -16968,10 +16965,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D24" s="6">
         <v>6.6257919999999998E-2</v>
@@ -17075,7 +17072,7 @@
         <v>15</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="6">
         <v>5.7877100000000001E-2</v>
@@ -17179,7 +17176,7 @@
         <v>46</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D26" s="6">
         <v>0.05</v>
@@ -17283,7 +17280,7 @@
         <v>47</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D27" s="6">
         <v>0.05</v>
@@ -17387,7 +17384,7 @@
         <v>48</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D28" s="6">
         <v>0.05</v>

</xml_diff>

<commit_message>
Add official deterministic TEMOA and +r reserve marg
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCA6500-676B-4674-9BFC-8E98B76431FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A58E9EC-07C8-4AFB-A4B9-CBCD6699FC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="13020" tabRatio="849" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodity_labels" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="231">
   <si>
     <t>p</t>
   </si>
@@ -603,9 +603,6 @@
     <t>maxact_notes</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>PJ</t>
   </si>
   <si>
@@ -748,15 +745,6 @@
   </si>
   <si>
     <t>stored Co2</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>GW</t>
   </si>
 </sst>
 </file>
@@ -769,7 +757,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -969,13 +957,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="MS Shell Dlg 2"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1009,12 +992,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1383,7 +1360,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1418,10 +1395,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="303">
@@ -2585,7 +2558,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B45" s="4">
         <v>0.64700000000000002</v>
@@ -2596,7 +2569,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B46" s="4">
         <v>0.64700000000000002</v>
@@ -2615,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0904B615-50FA-4F82-9A22-035234CBED38}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2639,7 +2612,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1">
         <v>0.17</v>
@@ -2658,7 +2631,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2754,393 +2727,35 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA9BB2C-9F9E-4D6B-AAF2-83D7B122A42E}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="7" width="15" style="15" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="15" t="s">
+      <c r="A1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="15">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="15">
-        <v>2025</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="15">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B4" s="15">
-        <v>2030</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="15">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B5" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="15">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="15">
-        <v>2040</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="15">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B7" s="15">
-        <v>2045</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="15">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="B8" s="15">
-        <v>2050</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="15">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B9" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="15">
-        <v>0</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B10" s="15">
-        <v>2025</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B11" s="15">
-        <v>2030</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="15">
-        <v>0</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="15">
-        <v>0</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B13" s="15">
-        <v>2040</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B14" s="15">
-        <v>2045</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B15" s="15">
-        <v>2050</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B16" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B17" s="15">
-        <v>2025</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="15">
-        <v>0</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18" s="15">
-        <v>2030</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B19" s="15">
-        <v>2035</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="15">
-        <v>0</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B20" s="15">
-        <v>2040</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="15">
-        <v>0</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" s="15">
-        <v>2045</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="15">
-        <v>0</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B22" s="15">
-        <v>2050</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="15">
-        <v>0</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3154,7 +2769,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3225,142 +2840,142 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2">
         <v>2023</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D2">
         <v>124.06851712928901</v>
       </c>
       <c r="E2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" t="s">
         <v>184</v>
-      </c>
-      <c r="F2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>2025</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3">
         <v>124.06851712928901</v>
       </c>
       <c r="E3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" t="s">
         <v>184</v>
-      </c>
-      <c r="F3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4">
         <v>2030</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D4">
         <v>124.06851712928901</v>
       </c>
       <c r="E4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" t="s">
         <v>184</v>
-      </c>
-      <c r="F4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5">
         <v>2035</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D5">
         <v>124.06851712928901</v>
       </c>
       <c r="E5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" t="s">
         <v>184</v>
-      </c>
-      <c r="F5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6">
         <v>2040</v>
       </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D6">
         <v>124.06851712928901</v>
       </c>
       <c r="E6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" t="s">
         <v>184</v>
-      </c>
-      <c r="F6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7">
         <v>2045</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7">
         <v>124.06851712928901</v>
       </c>
       <c r="E7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" t="s">
         <v>184</v>
-      </c>
-      <c r="F7" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8">
         <v>2050</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8">
         <v>124.06851712928901</v>
       </c>
       <c r="E8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" t="s">
         <v>184</v>
-      </c>
-      <c r="F8" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3501,13 +3116,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3523,57 +3138,57 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3622,46 +3237,46 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>202</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3673,7 +3288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B94D054-32A6-4BDE-98D7-472A0F6D7282}">
   <dimension ref="A1:AL84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -3822,7 +3437,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>51</v>
@@ -3938,7 +3553,7 @@
         <v>28</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>51</v>
@@ -4054,7 +3669,7 @@
         <v>38</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>51</v>
@@ -4170,7 +3785,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>51</v>
@@ -4286,7 +3901,7 @@
         <v>43</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>51</v>
@@ -4402,7 +4017,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>51</v>
@@ -4518,7 +4133,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>51</v>
@@ -5660,7 +5275,7 @@
         <v>83</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>51</v>
@@ -5770,7 +5385,7 @@
         <v>84</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>51</v>
@@ -5880,7 +5495,7 @@
         <v>44</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>51</v>
@@ -5990,7 +5605,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>51</v>
@@ -6100,7 +5715,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>51</v>
@@ -6210,7 +5825,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>51</v>
@@ -6320,7 +5935,7 @@
         <v>39</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>51</v>
@@ -11818,10 +11433,10 @@
         <v>145</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G71" s="9" t="s">
         <v>51</v>
@@ -11962,13 +11577,13 @@
         <v>119</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G72" s="9" t="s">
         <v>51</v>
@@ -12106,19 +11721,19 @@
         <v>6</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H73" s="4">
         <v>1</v>
@@ -12222,13 +11837,13 @@
         <v>6</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>60</v>
@@ -12335,16 +11950,16 @@
         <v>6</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H75" s="4">
         <v>1</v>
@@ -12448,16 +12063,16 @@
         <v>6</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H76" s="4">
         <v>1</v>
@@ -12561,16 +12176,16 @@
         <v>6</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H77" s="4">
         <v>1</v>
@@ -12674,16 +12289,16 @@
         <v>6</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H78" s="4">
         <v>1</v>
@@ -12787,16 +12402,16 @@
         <v>6</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H79" s="4">
         <v>1</v>
@@ -12900,13 +12515,13 @@
         <v>6</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>56</v>
@@ -13013,13 +12628,13 @@
         <v>6</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>53</v>
@@ -13126,13 +12741,13 @@
         <v>6</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>62</v>
@@ -13239,13 +12854,13 @@
         <v>6</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>58</v>
@@ -13352,16 +12967,16 @@
         <v>6</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H84" s="4">
         <v>1</v>
@@ -13507,7 +13122,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>118</v>
@@ -13516,7 +13131,7 @@
         <v>118.6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -13524,7 +13139,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>118</v>
@@ -13533,7 +13148,7 @@
         <v>118.62</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -13541,7 +13156,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>118</v>
@@ -13550,7 +13165,7 @@
         <v>118.62</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -13558,7 +13173,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>118</v>
@@ -13567,7 +13182,7 @@
         <v>202.32</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -13575,7 +13190,7 @@
         <v>120</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>118</v>
@@ -13584,7 +13199,7 @@
         <v>119.41764496915395</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -13592,7 +13207,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>118</v>
@@ -13601,7 +13216,7 @@
         <v>119.41764496915395</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -13609,7 +13224,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>118</v>
@@ -13618,7 +13233,7 @@
         <v>119.41764496915395</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -13626,7 +13241,7 @@
         <v>121</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>118</v>
@@ -13635,7 +13250,7 @@
         <v>229.51879128207057</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -13643,7 +13258,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>118</v>
@@ -13652,7 +13267,7 @@
         <v>229.51879128207057</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -13660,7 +13275,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>118</v>
@@ -13669,7 +13284,7 @@
         <v>229.51879128207057</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -13677,7 +13292,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>118</v>
@@ -13686,7 +13301,7 @@
         <v>214.12654767006592</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -13694,7 +13309,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>118</v>
@@ -13708,7 +13323,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>118</v>
@@ -13722,7 +13337,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>118</v>
@@ -13736,7 +13351,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>118</v>
@@ -13750,7 +13365,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>118</v>
@@ -13764,7 +13379,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>118</v>
@@ -13778,7 +13393,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>118</v>
@@ -13792,7 +13407,7 @@
         <v>109</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>118</v>
@@ -13802,7 +13417,7 @@
         <v>5.93</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -13810,7 +13425,7 @@
         <v>109</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>118</v>
@@ -13820,7 +13435,7 @@
         <v>112.66999999999999</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -13828,7 +13443,7 @@
         <v>110</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>118</v>
@@ -13838,7 +13453,7 @@
         <v>5.93</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -13846,7 +13461,7 @@
         <v>110</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>118</v>
@@ -13856,7 +13471,7 @@
         <v>112.66999999999999</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -13864,7 +13479,7 @@
         <v>111</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>118</v>
@@ -13874,7 +13489,7 @@
         <v>3.5579999999999998</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -13882,7 +13497,7 @@
         <v>111</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>118</v>
@@ -13892,7 +13507,7 @@
         <v>115.04199999999999</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -13900,7 +13515,7 @@
         <v>112</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>118</v>
@@ -13910,7 +13525,7 @@
         <v>3.5579999999999998</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K26" s="13"/>
     </row>
@@ -13919,7 +13534,7 @@
         <v>112</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>118</v>
@@ -13929,7 +13544,7 @@
         <v>115.04199999999999</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -13937,7 +13552,7 @@
         <v>113</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>118</v>
@@ -13947,7 +13562,7 @@
         <v>10.116</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K28" s="13"/>
     </row>
@@ -13956,7 +13571,7 @@
         <v>113</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>118</v>
@@ -13966,7 +13581,7 @@
         <v>192.20399999999998</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -13974,7 +13589,7 @@
         <v>114</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>118</v>
@@ -13984,7 +13599,7 @@
         <v>2.0232000000000001</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -13992,7 +13607,7 @@
         <v>114</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>118</v>
@@ -14002,15 +13617,15 @@
         <v>200.29679999999999</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>118</v>
@@ -14021,10 +13636,10 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>118</v>
@@ -14034,15 +13649,15 @@
         <v>-170.07300000000001</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>118</v>
@@ -14052,24 +13667,24 @@
         <v>170.07300000000001</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D35" s="6">
         <v>-1</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -14564,7 +14179,7 @@
         <v>2030</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D2" s="1">
         <v>26505.0756</v>
@@ -14584,7 +14199,7 @@
         <v>2035</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="1">
         <v>26505.0756</v>
@@ -14604,7 +14219,7 @@
         <v>2040</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="1">
         <v>26505.0756</v>
@@ -14624,7 +14239,7 @@
         <v>2045</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" s="1">
         <v>26505.0756</v>
@@ -14644,7 +14259,7 @@
         <v>2050</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -14664,7 +14279,7 @@
         <v>2023</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -14673,7 +14288,7 @@
         <v>147</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -14684,7 +14299,7 @@
         <v>2025</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -14693,7 +14308,7 @@
         <v>147</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -14704,7 +14319,7 @@
         <v>2030</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -14713,7 +14328,7 @@
         <v>147</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -14724,7 +14339,7 @@
         <v>2035</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -14733,7 +14348,7 @@
         <v>147</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -14744,7 +14359,7 @@
         <v>2040</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -14753,7 +14368,7 @@
         <v>147</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -14764,7 +14379,7 @@
         <v>2045</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -14773,7 +14388,7 @@
         <v>147</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -14784,7 +14399,7 @@
         <v>2050</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -14793,7 +14408,7 @@
         <v>147</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -20050,10 +19665,10 @@
         <v>6</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D28" s="6">
         <v>0.05</v>
@@ -20154,10 +19769,10 @@
         <v>6</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D29" s="6">
         <v>0.05</v>
@@ -20258,10 +19873,10 @@
         <v>6</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D30" s="6">
         <v>0.05</v>
@@ -20362,10 +19977,10 @@
         <v>6</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D31" s="6">
         <v>0.05</v>
@@ -20466,10 +20081,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D32" s="6">
         <v>0.05</v>
@@ -20570,10 +20185,10 @@
         <v>6</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D33" s="6">
         <v>0.05</v>
@@ -20674,10 +20289,10 @@
         <v>6</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D34" s="6">
         <v>0.05</v>
@@ -20778,10 +20393,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D35" s="6">
         <v>0.05</v>
@@ -20882,10 +20497,10 @@
         <v>6</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D36" s="6">
         <v>0.05</v>
@@ -20986,10 +20601,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D37" s="6">
         <v>0.05</v>
@@ -21090,10 +20705,10 @@
         <v>6</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" s="6">
         <v>0.05</v>
@@ -21194,10 +20809,10 @@
         <v>6</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D39" s="6">
         <v>0.05</v>
@@ -21298,7 +20913,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>141</v>
@@ -21402,7 +21017,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>141</v>

</xml_diff>